<commit_message>
CSS Verbesserungen, neue Buttons, Tabelle Streifen
</commit_message>
<xml_diff>
--- a/PythonCode/mysite/output.xlsx
+++ b/PythonCode/mysite/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="39">
   <si>
     <t>Vornamen</t>
   </si>
@@ -31,31 +31,37 @@
     <t>Verlassen</t>
   </si>
   <si>
+    <t>Stephan</t>
+  </si>
+  <si>
     <t>Eli</t>
   </si>
   <si>
-    <t>Steve</t>
-  </si>
-  <si>
-    <t>Stephan</t>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Detlef</t>
+  </si>
+  <si>
+    <t>Fuchs</t>
   </si>
   <si>
     <t>Enders</t>
   </si>
   <si>
-    <t>Mustermann</t>
-  </si>
-  <si>
-    <t>Fuchs</t>
+    <t>Schmitz</t>
+  </si>
+  <si>
+    <t>Soost</t>
+  </si>
+  <si>
+    <t>3C</t>
   </si>
   <si>
     <t>4a</t>
   </si>
   <si>
-    <t>10x</t>
-  </si>
-  <si>
-    <t>3C</t>
+    <t>1a</t>
   </si>
   <si>
     <t>10.03.2023 19:12</t>
@@ -88,6 +94,24 @@
     <t>10.13.2023 19:09</t>
   </si>
   <si>
+    <t>10.14.2023 20:28</t>
+  </si>
+  <si>
+    <t>10.14.2023 20:59</t>
+  </si>
+  <si>
+    <t>10.15.2023 18:18</t>
+  </si>
+  <si>
+    <t>10.17.2023 18:56</t>
+  </si>
+  <si>
+    <t>10.17.2023 18:58</t>
+  </si>
+  <si>
+    <t>10.17.2023 19:16</t>
+  </si>
+  <si>
     <t>10.03.2023 20:01</t>
   </si>
   <si>
@@ -101,6 +125,12 @@
   </si>
   <si>
     <t>10.13.2023 19:10</t>
+  </si>
+  <si>
+    <t>10.15.2023 20:05</t>
+  </si>
+  <si>
+    <t>10.17.2023 19:57</t>
   </si>
 </sst>
 </file>
@@ -458,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,16 +516,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -503,16 +533,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -520,67 +550,67 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -588,101 +618,220 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
         <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ExcelExport korrigiert, Buttons verschoben
</commit_message>
<xml_diff>
--- a/PythonCode/mysite/output.xlsx
+++ b/PythonCode/mysite/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="66">
   <si>
     <t>Vornamen</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Verlassen</t>
   </si>
   <si>
-    <t>DauerStunden</t>
+    <t>DauerMinuten</t>
   </si>
   <si>
     <t>Stephan</t>
@@ -139,6 +139,42 @@
     <t>12.11.2023 14:08</t>
   </si>
   <si>
+    <t>13.11.2023 21:49</t>
+  </si>
+  <si>
+    <t>13.11.2023 21:51</t>
+  </si>
+  <si>
+    <t>13.11.2023 21:58</t>
+  </si>
+  <si>
+    <t>14.11.2023 17:29</t>
+  </si>
+  <si>
+    <t>19.11.2023 18:54</t>
+  </si>
+  <si>
+    <t>19.11.2023 19:35</t>
+  </si>
+  <si>
+    <t>22.11.2023 10:32</t>
+  </si>
+  <si>
+    <t>22.11.2023 13:53</t>
+  </si>
+  <si>
+    <t>26.11.2023 16:02</t>
+  </si>
+  <si>
+    <t>07.12.2023 20:40</t>
+  </si>
+  <si>
+    <t>17.12.2023 22:06</t>
+  </si>
+  <si>
+    <t>18.12.2023 08:00</t>
+  </si>
+  <si>
     <t>03.10.2023 20:01</t>
   </si>
   <si>
@@ -164,6 +200,18 @@
   </si>
   <si>
     <t>12.11.2023 14:11</t>
+  </si>
+  <si>
+    <t>19.11.2023 19:34</t>
+  </si>
+  <si>
+    <t>07.12.2023 20:41</t>
+  </si>
+  <si>
+    <t>18.12.2023 08:08</t>
+  </si>
+  <si>
+    <t>18.12.2023 08:01</t>
   </si>
 </sst>
 </file>
@@ -521,7 +569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,7 +609,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F2">
         <v>49</v>
@@ -581,7 +629,7 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F3">
         <v>45</v>
@@ -601,7 +649,7 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>44</v>
@@ -641,7 +689,7 @@
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <v>93</v>
@@ -661,7 +709,7 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F7">
         <v>93</v>
@@ -761,7 +809,7 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F12">
         <v>16</v>
@@ -781,7 +829,7 @@
         <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -861,7 +909,7 @@
         <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F17">
         <v>107</v>
@@ -881,7 +929,7 @@
         <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="F18">
         <v>68</v>
@@ -901,7 +949,7 @@
         <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F19">
         <v>59</v>
@@ -921,7 +969,7 @@
         <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F20">
         <v>41</v>
@@ -981,7 +1029,7 @@
         <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="F23">
         <v>3</v>
@@ -1001,7 +1049,7 @@
         <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="F24">
         <v>16</v>
@@ -1021,7 +1069,7 @@
         <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="F25">
         <v>16</v>
@@ -1061,7 +1109,7 @@
         <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F27">
         <v>8</v>
@@ -1081,7 +1129,7 @@
         <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F28">
         <v>7</v>
@@ -1101,10 +1149,350 @@
         <v>40</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F29">
         <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" t="s">
+        <v>51</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" t="s">
+        <v>51</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>